<commit_message>
Okay, I've come to the conclusion that my forward kinematics works just fine, it just can't do angles that match the system ones lmao. Worth continuing.
</commit_message>
<xml_diff>
--- a/DH-Transformation_UR3e.xlsx
+++ b/DH-Transformation_UR3e.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odonnell_Lab\Documents\Ben_Anderson_Robot_stuff\COBOT-Transducer-Control-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A76D06-DDBE-40D6-B697-621006A3A192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE674867-4410-44FB-9BD8-1A88DFF0FADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,6 +711,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -752,30 +776,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,19 +833,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.24354999999999999</c:v>
+                  <c:v>4.4757735928949161E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,19 +860,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.491924530964972E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.7979327838975612E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.22315000000000002</c:v>
+                  <c:v>-0.22314999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,19 +922,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.24354999999999999</c:v>
+                  <c:v>4.4757735928949161E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,19 +949,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.491924530964972E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.7979327838975612E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.22315000000000002</c:v>
+                  <c:v>-0.22314999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1142,19 +1142,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.24354999999999999</c:v>
+                  <c:v>4.4757735928949161E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>8.3937983516926837E-17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.45674999999999999</c:v>
+                  <c:v>1.1530790970486207E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1169,19 +1169,19 @@
                   <c:v>0.15185000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.39539999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.60860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.60860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6500000000000017E-2</c:v>
+                  <c:v>0.69395000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6500000000000017E-2</c:v>
+                  <c:v>0.69395000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,19 +1360,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.491924530964972E-17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.7979327838975612E-17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.13105</c:v>
+                  <c:v>-0.13104999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.22315000000000002</c:v>
+                  <c:v>-0.22314999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,19 +1387,19 @@
                   <c:v>0.15185000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.39539999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.60860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15185000000000001</c:v>
+                  <c:v>0.60860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6500000000000017E-2</c:v>
+                  <c:v>0.69395000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6500000000000017E-2</c:v>
+                  <c:v>0.69395000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,7 +1525,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="20" fmlaLink="$N$7" horiz="1" max="360" page="10" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="20" fmlaLink="$N$7" horiz="1" max="360" page="10" val="270"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1537,7 +1537,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="20" fmlaLink="$N$9" horiz="1" max="360" page="10" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="20" fmlaLink="$N$9" horiz="1" max="360" page="10" val="270"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3335,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F1:AQ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,38 +3351,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="O1" s="85" t="s">
+      <c r="O1" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
     </row>
     <row r="2" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="O2" s="86" t="s">
+      <c r="O2" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
     </row>
     <row r="3" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
     </row>
     <row r="4" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="M4" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
+      <c r="M4" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
     </row>
     <row r="5" spans="6:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M5" s="15" t="s">
@@ -3436,11 +3436,11 @@
         <v>9</v>
       </c>
       <c r="N7" s="21">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="O7" s="22">
         <f t="shared" ref="O7:O11" si="0">RADIANS(N7)</f>
-        <v>0</v>
+        <v>4.7123889803846897</v>
       </c>
       <c r="P7" s="23">
         <v>-0.24354999999999999</v>
@@ -3487,11 +3487,11 @@
         <v>11</v>
       </c>
       <c r="N9" s="29">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="O9" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.7123889803846897</v>
       </c>
       <c r="P9" s="31">
         <v>0</v>
@@ -3561,19 +3561,19 @@
       </c>
     </row>
     <row r="12" spans="6:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F12" s="88" t="s">
+      <c r="F12" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="89" t="s">
+      <c r="G12" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="92" t="s">
+      <c r="H12" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="91" t="s">
+      <c r="I12" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="90" t="s">
+      <c r="J12" s="76" t="s">
         <v>33</v>
       </c>
       <c r="K12" s="43" t="s">
@@ -3581,11 +3581,11 @@
       </c>
     </row>
     <row r="13" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="88"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="90"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="76"/>
       <c r="K13" s="2"/>
       <c r="L13" s="69"/>
       <c r="M13" s="69"/>
@@ -3600,11 +3600,11 @@
       <c r="X13" s="40"/>
     </row>
     <row r="14" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F14" s="88"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="90"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="76"/>
       <c r="K14" s="2"/>
       <c r="L14" s="69"/>
       <c r="M14" s="69"/>
@@ -3619,26 +3619,26 @@
       <c r="X14" s="40"/>
     </row>
     <row r="15" spans="6:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="88"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="90"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="76"/>
       <c r="K15" s="2"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="84" t="s">
+      <c r="M15" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="84"/>
-      <c r="O15" s="84"/>
-      <c r="P15" s="84"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="92"/>
     </row>
     <row r="16" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F16" s="88"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="90"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="76"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="1">
@@ -3660,13 +3660,13 @@
       <c r="Q16" s="14"/>
     </row>
     <row r="17" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F17" s="88"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="90"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="76"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="82"/>
+      <c r="L17" s="90"/>
       <c r="M17" s="1">
         <f>SIN(O6)</f>
         <v>0</v>
@@ -3686,13 +3686,13 @@
       <c r="Q17" s="14"/>
     </row>
     <row r="18" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F18" s="88"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="91"/>
-      <c r="J18" s="90"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="76"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="82"/>
+      <c r="L18" s="90"/>
       <c r="M18" s="1">
         <v>0</v>
       </c>
@@ -3711,11 +3711,11 @@
       <c r="Q18" s="14"/>
     </row>
     <row r="19" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F19" s="88"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="90"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="76"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="1">
@@ -3733,11 +3733,11 @@
       <c r="Q19" s="14"/>
     </row>
     <row r="20" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F20" s="88"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="90"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="76"/>
       <c r="Q20" s="14"/>
       <c r="R20" s="14"/>
       <c r="S20" s="46"/>
@@ -3745,10 +3745,10 @@
       <c r="U20" s="47"/>
     </row>
     <row r="21" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F21" s="88"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="92"/>
-      <c r="I21" s="91"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="77"/>
       <c r="J21" s="3"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -3763,10 +3763,10 @@
       <c r="U21" s="47"/>
     </row>
     <row r="22" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F22" s="88"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="91"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="77"/>
       <c r="J22" s="3"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
@@ -3781,19 +3781,19 @@
       <c r="U22" s="47"/>
     </row>
     <row r="23" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="91"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="77"/>
       <c r="J23" s="3"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="84" t="s">
+      <c r="M23" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="84"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="84"/>
+      <c r="N23" s="92"/>
+      <c r="O23" s="92"/>
+      <c r="P23" s="92"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="47"/>
       <c r="S23" s="46"/>
@@ -3801,20 +3801,20 @@
       <c r="U23" s="47"/>
     </row>
     <row r="24" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F24" s="88"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="91"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="77"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="4">
         <f>COS(O7)</f>
-        <v>1</v>
+        <v>-1.83772268236293E-16</v>
       </c>
       <c r="N24" s="4">
         <f>-(SIN(O7))*COS(R7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="4">
         <f>SIN(O7)*SIN(R7)</f>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="P24" s="4">
         <f>P7*COS(O7)</f>
-        <v>-0.24354999999999999</v>
+        <v>4.4757735928949161E-17</v>
       </c>
       <c r="Q24" s="14"/>
       <c r="R24" s="48"/>
@@ -3831,33 +3831,33 @@
       <c r="U24" s="49"/>
       <c r="V24" s="50">
         <f t="array" ref="V24:Y27">MMULT(M16:P19,M24:P27)</f>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="W24" s="50">
         <v>1</v>
       </c>
-      <c r="W24" s="50">
-        <v>0</v>
-      </c>
       <c r="X24" s="50">
         <v>0</v>
       </c>
       <c r="Y24" s="52">
-        <v>-0.24354999999999999</v>
+        <v>4.4757735928949161E-17</v>
       </c>
     </row>
     <row r="25" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F25" s="88"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="91"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="77"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="4">
         <f>SIN(O7)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N25" s="4">
         <f>COS(O7)*COS(R7)</f>
-        <v>1</v>
+        <v>-1.83772268236293E-16</v>
       </c>
       <c r="O25" s="4">
         <f>-(COS(O7))*SIN(R7)</f>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="P25" s="4">
         <f>P7*SIN(O7)</f>
-        <v>0</v>
+        <v>0.24354999999999999</v>
       </c>
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
@@ -3873,23 +3873,23 @@
       <c r="T25" s="47"/>
       <c r="U25" s="49"/>
       <c r="V25" s="50">
-        <v>0</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="W25" s="50">
-        <v>6.1257422745431001E-17</v>
+        <v>-1.1257415524237342E-32</v>
       </c>
       <c r="X25" s="50">
         <v>-1</v>
       </c>
       <c r="Y25" s="53">
-        <v>0</v>
+        <v>1.491924530964972E-17</v>
       </c>
     </row>
     <row r="26" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F26" s="88"/>
-      <c r="G26" s="89"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="91"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="77"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -3914,23 +3914,23 @@
       <c r="T26" s="47"/>
       <c r="U26" s="49"/>
       <c r="V26" s="50">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W26" s="50">
-        <v>1</v>
+        <v>-1.83772268236293E-16</v>
       </c>
       <c r="X26" s="50">
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="Y26" s="54">
-        <v>0.15185000000000001</v>
+        <v>0.39539999999999997</v>
       </c>
     </row>
     <row r="27" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F27" s="88"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="91"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="77"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -3965,10 +3965,10 @@
       </c>
     </row>
     <row r="28" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F28" s="88"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="91"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="77"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
@@ -3980,9 +3980,9 @@
       <c r="Y28" s="51"/>
     </row>
     <row r="29" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F29" s="88"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="92"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="78"/>
       <c r="I29" s="42"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -4002,9 +4002,9 @@
       <c r="Y29" s="51"/>
     </row>
     <row r="30" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="92"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="78"/>
       <c r="I30" s="5"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -4024,19 +4024,19 @@
       <c r="Y30" s="51"/>
     </row>
     <row r="31" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F31" s="88"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="92"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="78"/>
       <c r="I31" s="5"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="84" t="s">
+      <c r="M31" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="N31" s="84"/>
-      <c r="O31" s="84"/>
-      <c r="P31" s="84"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="92"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
@@ -4048,9 +4048,9 @@
       <c r="Y31" s="51"/>
     </row>
     <row r="32" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F32" s="88"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="92"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="78"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -4078,22 +4078,22 @@
       <c r="U32" s="14"/>
       <c r="V32" s="50">
         <f t="array" ref="V32:Y35">MMULT(V24:Y27,M32:P35)</f>
+        <v>-1.83772268236293E-16</v>
+      </c>
+      <c r="W32" s="50">
         <v>1</v>
       </c>
-      <c r="W32" s="50">
-        <v>0</v>
-      </c>
       <c r="X32" s="50">
         <v>0</v>
       </c>
       <c r="Y32" s="52">
-        <v>-0.45674999999999999</v>
+        <v>8.3937983516926837E-17</v>
       </c>
     </row>
     <row r="33" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="92"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="78"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -4120,22 +4120,22 @@
       <c r="T33" s="14"/>
       <c r="U33" s="14"/>
       <c r="V33" s="50">
-        <v>0</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="W33" s="50">
-        <v>6.1257422745431001E-17</v>
+        <v>-1.1257415524237342E-32</v>
       </c>
       <c r="X33" s="50">
         <v>-1</v>
       </c>
       <c r="Y33" s="53">
-        <v>0</v>
+        <v>2.7979327838975612E-17</v>
       </c>
     </row>
     <row r="34" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F34" s="88"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="92"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="78"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -4161,22 +4161,22 @@
       <c r="T34" s="14"/>
       <c r="U34" s="14"/>
       <c r="V34" s="50">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W34" s="50">
-        <v>1</v>
+        <v>-1.83772268236293E-16</v>
       </c>
       <c r="X34" s="50">
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="Y34" s="54">
-        <v>0.15185000000000001</v>
+        <v>0.60860000000000003</v>
       </c>
     </row>
     <row r="35" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F35" s="88"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="92"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="78"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -4212,17 +4212,17 @@
       </c>
     </row>
     <row r="36" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="92"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="78"/>
       <c r="V36" s="51"/>
       <c r="W36" s="51"/>
       <c r="X36" s="51"/>
       <c r="Y36" s="51"/>
     </row>
     <row r="37" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="88"/>
-      <c r="G37" s="89"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="75"/>
       <c r="H37" s="7"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
@@ -4238,8 +4238,8 @@
       <c r="Y37" s="51"/>
     </row>
     <row r="38" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F38" s="88"/>
-      <c r="G38" s="89"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="75"/>
       <c r="H38" s="7"/>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -4262,34 +4262,34 @@
       <c r="AD38" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="AG38" s="71" t="s">
+      <c r="AG38" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="AH38" s="72"/>
-      <c r="AI38" s="72"/>
-      <c r="AJ38" s="72"/>
-      <c r="AK38" s="72"/>
-      <c r="AL38" s="72"/>
-      <c r="AM38" s="72"/>
-      <c r="AN38" s="72"/>
-      <c r="AO38" s="72"/>
-      <c r="AP38" s="72"/>
-      <c r="AQ38" s="73"/>
+      <c r="AH38" s="80"/>
+      <c r="AI38" s="80"/>
+      <c r="AJ38" s="80"/>
+      <c r="AK38" s="80"/>
+      <c r="AL38" s="80"/>
+      <c r="AM38" s="80"/>
+      <c r="AN38" s="80"/>
+      <c r="AO38" s="80"/>
+      <c r="AP38" s="80"/>
+      <c r="AQ38" s="81"/>
     </row>
     <row r="39" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="75"/>
       <c r="H39" s="7"/>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="84" t="s">
+      <c r="M39" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="N39" s="84"/>
-      <c r="O39" s="84"/>
-      <c r="P39" s="84"/>
+      <c r="N39" s="92"/>
+      <c r="O39" s="92"/>
+      <c r="P39" s="92"/>
       <c r="V39" s="51"/>
       <c r="W39" s="51"/>
       <c r="X39" s="51"/>
@@ -4306,21 +4306,21 @@
         <f>P18</f>
         <v>0.15185000000000001</v>
       </c>
-      <c r="AG39" s="74"/>
-      <c r="AH39" s="75"/>
-      <c r="AI39" s="75"/>
-      <c r="AJ39" s="75"/>
-      <c r="AK39" s="75"/>
-      <c r="AL39" s="75"/>
-      <c r="AM39" s="75"/>
-      <c r="AN39" s="75"/>
-      <c r="AO39" s="75"/>
-      <c r="AP39" s="75"/>
-      <c r="AQ39" s="76"/>
+      <c r="AG39" s="82"/>
+      <c r="AH39" s="83"/>
+      <c r="AI39" s="83"/>
+      <c r="AJ39" s="83"/>
+      <c r="AK39" s="83"/>
+      <c r="AL39" s="83"/>
+      <c r="AM39" s="83"/>
+      <c r="AN39" s="83"/>
+      <c r="AO39" s="83"/>
+      <c r="AP39" s="83"/>
+      <c r="AQ39" s="84"/>
     </row>
     <row r="40" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F40" s="88"/>
-      <c r="G40" s="89"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="75"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
@@ -4328,15 +4328,15 @@
       <c r="L40" s="7"/>
       <c r="M40" s="8">
         <f>COS(O9)</f>
-        <v>1</v>
+        <v>-1.83772268236293E-16</v>
       </c>
       <c r="N40" s="8">
         <f>-(SIN(O9))*COS(R9)</f>
-        <v>0</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="O40" s="8">
         <f>SIN(O9)*SIN(R9)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P40" s="8">
         <f>P9*COS(O9)</f>
@@ -4344,44 +4344,44 @@
       </c>
       <c r="V40" s="50">
         <f t="array" ref="V40:Y43">MMULT(V32:Y35,M40:P43)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W40" s="50">
-        <v>0</v>
+        <v>-2.2514831048474684E-32</v>
       </c>
       <c r="X40" s="50">
-        <v>0</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="Y40" s="52">
-        <v>-0.45674999999999999</v>
+        <v>8.3937983516926837E-17</v>
       </c>
       <c r="AB40" s="56">
         <f>Y24</f>
-        <v>-0.24354999999999999</v>
+        <v>4.4757735928949161E-17</v>
       </c>
       <c r="AC40" s="56">
         <f>Y25</f>
-        <v>0</v>
+        <v>1.491924530964972E-17</v>
       </c>
       <c r="AD40" s="56">
         <f>Y26</f>
-        <v>0.15185000000000001</v>
-      </c>
-      <c r="AG40" s="74"/>
-      <c r="AH40" s="75"/>
-      <c r="AI40" s="75"/>
-      <c r="AJ40" s="75"/>
-      <c r="AK40" s="75"/>
-      <c r="AL40" s="75"/>
-      <c r="AM40" s="75"/>
-      <c r="AN40" s="75"/>
-      <c r="AO40" s="75"/>
-      <c r="AP40" s="75"/>
-      <c r="AQ40" s="76"/>
+        <v>0.39539999999999997</v>
+      </c>
+      <c r="AG40" s="82"/>
+      <c r="AH40" s="83"/>
+      <c r="AI40" s="83"/>
+      <c r="AJ40" s="83"/>
+      <c r="AK40" s="83"/>
+      <c r="AL40" s="83"/>
+      <c r="AM40" s="83"/>
+      <c r="AN40" s="83"/>
+      <c r="AO40" s="83"/>
+      <c r="AP40" s="83"/>
+      <c r="AQ40" s="84"/>
     </row>
     <row r="41" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F41" s="88"/>
-      <c r="G41" s="89"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="75"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
@@ -4389,59 +4389,59 @@
       <c r="L41" s="7"/>
       <c r="M41" s="8">
         <f>SIN(O9)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N41" s="8">
         <f>COS(O9)*COS(R9)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-1.1257415524237342E-32</v>
       </c>
       <c r="O41" s="8">
         <f>-(COS(O9))*SIN(R9)</f>
-        <v>-1</v>
+        <v>1.83772268236293E-16</v>
       </c>
       <c r="P41" s="8">
         <f>P9*SIN(O9)</f>
         <v>0</v>
       </c>
       <c r="V41" s="50">
-        <v>0</v>
+        <v>2.2514831048474684E-32</v>
       </c>
       <c r="W41" s="50">
         <v>-1</v>
       </c>
       <c r="X41" s="50">
-        <v>-1.22514845490862E-16</v>
+        <v>0</v>
       </c>
       <c r="Y41" s="53">
-        <v>-0.13105</v>
+        <v>-0.13104999999999997</v>
       </c>
       <c r="AB41" s="56">
         <f>Y32</f>
-        <v>-0.45674999999999999</v>
+        <v>8.3937983516926837E-17</v>
       </c>
       <c r="AC41" s="56">
         <f>Y33</f>
-        <v>0</v>
+        <v>2.7979327838975612E-17</v>
       </c>
       <c r="AD41" s="56">
         <f>Y34</f>
-        <v>0.15185000000000001</v>
-      </c>
-      <c r="AG41" s="74"/>
-      <c r="AH41" s="75"/>
-      <c r="AI41" s="75"/>
-      <c r="AJ41" s="75"/>
-      <c r="AK41" s="75"/>
-      <c r="AL41" s="75"/>
-      <c r="AM41" s="75"/>
-      <c r="AN41" s="75"/>
-      <c r="AO41" s="75"/>
-      <c r="AP41" s="75"/>
-      <c r="AQ41" s="76"/>
+        <v>0.60860000000000003</v>
+      </c>
+      <c r="AG41" s="82"/>
+      <c r="AH41" s="83"/>
+      <c r="AI41" s="83"/>
+      <c r="AJ41" s="83"/>
+      <c r="AK41" s="83"/>
+      <c r="AL41" s="83"/>
+      <c r="AM41" s="83"/>
+      <c r="AN41" s="83"/>
+      <c r="AO41" s="83"/>
+      <c r="AP41" s="83"/>
+      <c r="AQ41" s="84"/>
     </row>
     <row r="42" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="75"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
@@ -4463,44 +4463,44 @@
         <v>0.13105</v>
       </c>
       <c r="V42" s="50">
-        <v>0</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="W42" s="50">
-        <v>1.22514845490862E-16</v>
+        <v>0</v>
       </c>
       <c r="X42" s="50">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y42" s="54">
-        <v>0.15185000000000001</v>
+        <v>0.60860000000000003</v>
       </c>
       <c r="AB42" s="56">
         <f>Y40</f>
-        <v>-0.45674999999999999</v>
+        <v>8.3937983516926837E-17</v>
       </c>
       <c r="AC42" s="56">
         <f>Y41</f>
-        <v>-0.13105</v>
+        <v>-0.13104999999999997</v>
       </c>
       <c r="AD42" s="56">
         <f>Y42</f>
-        <v>0.15185000000000001</v>
-      </c>
-      <c r="AG42" s="77"/>
-      <c r="AH42" s="78"/>
-      <c r="AI42" s="78"/>
-      <c r="AJ42" s="78"/>
-      <c r="AK42" s="78"/>
-      <c r="AL42" s="78"/>
-      <c r="AM42" s="78"/>
-      <c r="AN42" s="78"/>
-      <c r="AO42" s="78"/>
-      <c r="AP42" s="78"/>
-      <c r="AQ42" s="79"/>
+        <v>0.60860000000000003</v>
+      </c>
+      <c r="AG42" s="85"/>
+      <c r="AH42" s="86"/>
+      <c r="AI42" s="86"/>
+      <c r="AJ42" s="86"/>
+      <c r="AK42" s="86"/>
+      <c r="AL42" s="86"/>
+      <c r="AM42" s="86"/>
+      <c r="AN42" s="86"/>
+      <c r="AO42" s="86"/>
+      <c r="AP42" s="86"/>
+      <c r="AQ42" s="87"/>
     </row>
     <row r="43" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F43" s="88"/>
-      <c r="G43" s="89"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="75"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
@@ -4532,39 +4532,39 @@
       </c>
       <c r="AB43" s="56">
         <f>Y48</f>
-        <v>-0.45674999999999999</v>
+        <v>1.1530790970486207E-16</v>
       </c>
       <c r="AC43" s="56">
         <f>Y49</f>
-        <v>-0.13105</v>
+        <v>-0.13104999999999997</v>
       </c>
       <c r="AD43" s="56">
         <f>Y50</f>
-        <v>6.6500000000000017E-2</v>
+        <v>0.69395000000000007</v>
       </c>
     </row>
     <row r="44" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F44" s="88"/>
-      <c r="G44" s="89"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="75"/>
       <c r="V44" s="51"/>
       <c r="W44" s="51"/>
       <c r="X44" s="51"/>
       <c r="Y44" s="51"/>
       <c r="AB44" s="56">
         <f>Y56</f>
-        <v>-0.45674999999999999</v>
+        <v>1.1530790970486207E-16</v>
       </c>
       <c r="AC44" s="56">
         <f>Y57</f>
-        <v>-0.22315000000000002</v>
+        <v>-0.22314999999999996</v>
       </c>
       <c r="AD44" s="56">
         <f>Y58</f>
-        <v>6.6500000000000017E-2</v>
+        <v>0.69395000000000007</v>
       </c>
     </row>
     <row r="45" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F45" s="88"/>
+      <c r="F45" s="74"/>
       <c r="G45" s="10"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
@@ -4581,7 +4581,7 @@
       <c r="Y45" s="51"/>
     </row>
     <row r="46" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F46" s="88"/>
+      <c r="F46" s="74"/>
       <c r="G46" s="10"/>
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
@@ -4598,19 +4598,19 @@
       <c r="Y46" s="51"/>
     </row>
     <row r="47" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F47" s="88"/>
+      <c r="F47" s="74"/>
       <c r="G47" s="10"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
-      <c r="M47" s="84" t="s">
+      <c r="M47" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="N47" s="84"/>
-      <c r="O47" s="84"/>
-      <c r="P47" s="84"/>
+      <c r="N47" s="92"/>
+      <c r="O47" s="92"/>
+      <c r="P47" s="92"/>
       <c r="V47" s="51"/>
       <c r="W47" s="51"/>
       <c r="X47" s="51"/>
@@ -4626,7 +4626,7 @@
       </c>
     </row>
     <row r="48" spans="6:43" x14ac:dyDescent="0.25">
-      <c r="F48" s="88"/>
+      <c r="F48" s="74"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -4651,20 +4651,20 @@
       </c>
       <c r="V48" s="50">
         <f t="array" ref="V48:Y51">MMULT(V40:Y43,M48:P51)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W48" s="50">
-        <v>0</v>
+        <v>-3.67544536472586E-16</v>
       </c>
       <c r="X48" s="50">
         <v>0</v>
       </c>
       <c r="Y48" s="52">
-        <v>-0.45674999999999999</v>
+        <v>1.1530790970486207E-16</v>
       </c>
       <c r="AB48" s="56">
         <f>ATAN2(-V58,SQRT(POWER(V56,2)+POWER(V57,2)))</f>
-        <v>1.5707963267948966</v>
+        <v>1.5707963267948968</v>
       </c>
       <c r="AC48" s="56">
         <f>ATAN2(V57/COS(AB48),V56/COS(AB48))</f>
@@ -4672,11 +4672,11 @@
       </c>
       <c r="AD48" s="56">
         <f>ATAN2(W58/COS(AB48),X58/COS(AB48))</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
     </row>
     <row r="49" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F49" s="88"/>
+      <c r="F49" s="74"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
@@ -4700,20 +4700,20 @@
         <v>0</v>
       </c>
       <c r="V49" s="50">
-        <v>0</v>
+        <v>2.2514831048474684E-32</v>
       </c>
       <c r="W49" s="50">
-        <v>6.1257422745431001E-17</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="X49" s="50">
         <v>-1</v>
       </c>
       <c r="Y49" s="53">
-        <v>-0.13105</v>
+        <v>-0.13104999999999997</v>
       </c>
       <c r="AB49" s="56">
         <f>DEGREES(AB48)</f>
-        <v>90</v>
+        <v>90.000000000000014</v>
       </c>
       <c r="AC49" s="56">
         <f>DEGREES(AC48)</f>
@@ -4721,11 +4721,11 @@
       </c>
       <c r="AD49" s="56">
         <f>DEGREES(AD48)</f>
-        <v>3.5097917871618886E-15</v>
+        <v>-3.5097917871618886E-15</v>
       </c>
     </row>
     <row r="50" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F50" s="88"/>
+      <c r="F50" s="74"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
@@ -4748,20 +4748,20 @@
         <v>8.5349999999999995E-2</v>
       </c>
       <c r="V50" s="50">
-        <v>0</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="W50" s="50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X50" s="50">
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="Y50" s="54">
-        <v>6.6500000000000017E-2</v>
+        <v>0.69395000000000007</v>
       </c>
     </row>
     <row r="51" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F51" s="88"/>
+      <c r="F51" s="74"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
@@ -4794,7 +4794,7 @@
       </c>
     </row>
     <row r="52" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F52" s="88"/>
+      <c r="F52" s="74"/>
       <c r="V52" s="51"/>
       <c r="W52" s="51"/>
       <c r="X52" s="51"/>
@@ -4844,12 +4844,12 @@
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
-      <c r="M55" s="80" t="s">
+      <c r="M55" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="N55" s="81"/>
-      <c r="O55" s="81"/>
-      <c r="P55" s="81"/>
+      <c r="N55" s="89"/>
+      <c r="O55" s="89"/>
+      <c r="P55" s="89"/>
       <c r="V55" s="51"/>
       <c r="W55" s="51"/>
       <c r="X55" s="51"/>
@@ -4881,16 +4881,16 @@
       </c>
       <c r="V56" s="61">
         <f t="array" ref="V56:Y59">MMULT(V48:Y51,M56:P59)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W56" s="62">
-        <v>0</v>
+        <v>-3.67544536472586E-16</v>
       </c>
       <c r="X56" s="63">
         <v>0</v>
       </c>
       <c r="Y56" s="57">
-        <v>-0.45674999999999999</v>
+        <v>1.1530790970486207E-16</v>
       </c>
     </row>
     <row r="57" spans="6:30" x14ac:dyDescent="0.25">
@@ -4918,16 +4918,16 @@
         <v>0</v>
       </c>
       <c r="V57" s="64">
-        <v>0</v>
+        <v>2.2514831048474684E-32</v>
       </c>
       <c r="W57" s="50">
-        <v>6.1257422745431001E-17</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="X57" s="65">
         <v>-1</v>
       </c>
       <c r="Y57" s="58">
-        <v>-0.22315000000000002</v>
+        <v>-0.22314999999999996</v>
       </c>
     </row>
     <row r="58" spans="6:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4954,16 +4954,16 @@
         <v>9.2100000000000001E-2</v>
       </c>
       <c r="V58" s="66">
-        <v>0</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="W58" s="67">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X58" s="68">
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="Y58" s="59">
-        <v>6.6500000000000017E-2</v>
+        <v>0.69395000000000007</v>
       </c>
     </row>
     <row r="59" spans="6:30" x14ac:dyDescent="0.25">
@@ -5002,14 +5002,6 @@
     <row r="63" spans="6:30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="P2:R3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="F12:F52"/>
-    <mergeCell ref="G12:G44"/>
-    <mergeCell ref="J12:J20"/>
-    <mergeCell ref="I12:I28"/>
-    <mergeCell ref="H12:H36"/>
     <mergeCell ref="AG38:AQ42"/>
     <mergeCell ref="M55:P55"/>
     <mergeCell ref="L17:L18"/>
@@ -5019,6 +5011,14 @@
     <mergeCell ref="M31:P31"/>
     <mergeCell ref="M39:P39"/>
     <mergeCell ref="M47:P47"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="P2:R3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="F12:F52"/>
+    <mergeCell ref="G12:G44"/>
+    <mergeCell ref="J12:J20"/>
+    <mergeCell ref="I12:I28"/>
+    <mergeCell ref="H12:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>